<commit_message>
generating templates for each entity types
</commit_message>
<xml_diff>
--- a/spotcheck/spotcheck_df_curated_v1_entity.xlsx
+++ b/spotcheck/spotcheck_df_curated_v1_entity.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B202"/>
+  <dimension ref="A1:B187"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,7 +477,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Oman</t>
+          <t>Vietnam</t>
         </is>
       </c>
     </row>
@@ -489,7 +489,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Italy</t>
+          <t>Oman</t>
         </is>
       </c>
     </row>
@@ -501,7 +501,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Austria</t>
+          <t>Italy</t>
         </is>
       </c>
     </row>
@@ -513,7 +513,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Netherlands</t>
+          <t>United States</t>
         </is>
       </c>
     </row>
@@ -525,7 +525,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Russia</t>
         </is>
       </c>
     </row>
@@ -537,7 +537,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Russia</t>
+          <t>Sweden</t>
         </is>
       </c>
     </row>
@@ -549,7 +549,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Sweden</t>
+          <t>Norway</t>
         </is>
       </c>
     </row>
@@ -561,7 +561,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Norway</t>
+          <t>Malaysia</t>
         </is>
       </c>
     </row>
@@ -573,7 +573,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Malaysia</t>
+          <t>Switzerland</t>
         </is>
       </c>
     </row>
@@ -609,7 +609,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Poland</t>
+          <t>Romania</t>
         </is>
       </c>
     </row>
@@ -621,7 +621,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Nigeria</t>
+          <t>Poland</t>
         </is>
       </c>
     </row>
@@ -633,7 +633,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Portugal</t>
+          <t>Nigeria</t>
         </is>
       </c>
     </row>
@@ -645,7 +645,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Uganda</t>
+          <t>China</t>
         </is>
       </c>
     </row>
@@ -657,7 +657,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Thailand</t>
+          <t>Portugal</t>
         </is>
       </c>
     </row>
@@ -669,7 +669,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Kuwait</t>
+          <t>Australia</t>
         </is>
       </c>
     </row>
@@ -681,7 +681,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>Thailand</t>
         </is>
       </c>
     </row>
@@ -693,7 +693,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Belgium</t>
+          <t>Kuwait</t>
         </is>
       </c>
     </row>
@@ -705,7 +705,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>France</t>
         </is>
       </c>
     </row>
@@ -717,7 +717,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>Belgium</t>
         </is>
       </c>
     </row>
@@ -729,7 +729,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Algeria</t>
+          <t>Spain</t>
         </is>
       </c>
     </row>
@@ -741,7 +741,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Armenia</t>
+          <t>Turkey</t>
         </is>
       </c>
     </row>
@@ -753,7 +753,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Iran</t>
+          <t>Algeria</t>
         </is>
       </c>
     </row>
@@ -765,7 +765,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Egypt</t>
+          <t>Armenia</t>
         </is>
       </c>
     </row>
@@ -777,7 +777,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Iran</t>
         </is>
       </c>
     </row>
@@ -789,7 +789,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Israel</t>
+          <t>Egypt</t>
         </is>
       </c>
     </row>
@@ -801,7 +801,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Hungary</t>
+          <t>Denmark</t>
         </is>
       </c>
     </row>
@@ -813,7 +813,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Ghana</t>
+          <t>Israel</t>
         </is>
       </c>
     </row>
@@ -873,31 +873,31 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Greece</t>
+          <t>Iceland</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>Country</t>
+          <t>Creative Work</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Maldives</t>
+          <t>Memento</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>Country</t>
+          <t>Creative Work</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Iceland</t>
+          <t>Spirited Away</t>
         </is>
       </c>
     </row>
@@ -909,7 +909,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Gangnam Style</t>
+          <t>The Dark Knight</t>
         </is>
       </c>
     </row>
@@ -921,7 +921,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Imagine Dragons</t>
+          <t>Pulp Fiction</t>
         </is>
       </c>
     </row>
@@ -933,7 +933,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Life is Beautiful</t>
+          <t>A Separation</t>
         </is>
       </c>
     </row>
@@ -945,7 +945,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Into the Wild</t>
+          <t>Run Lola Run</t>
         </is>
       </c>
     </row>
@@ -957,7 +957,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>The Godfather: Part II</t>
+          <t>Amélie</t>
         </is>
       </c>
     </row>
@@ -969,7 +969,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Amélie</t>
+          <t>The Green Mile</t>
         </is>
       </c>
     </row>
@@ -981,7 +981,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>The Seventh Seal</t>
+          <t>War and Peace</t>
         </is>
       </c>
     </row>
@@ -993,7 +993,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Spirited Away</t>
+          <t>The Handmaid's Tale</t>
         </is>
       </c>
     </row>
@@ -1005,7 +1005,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Schindler's List</t>
+          <t>The Brothers Karamazov</t>
         </is>
       </c>
     </row>
@@ -1017,7 +1017,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>The Grapes of Wrath</t>
+          <t>Dracula</t>
         </is>
       </c>
     </row>
@@ -1029,7 +1029,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Brave New World</t>
+          <t>Pride and Prejudice</t>
         </is>
       </c>
     </row>
@@ -1041,7 +1041,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>The Lord of the Rings</t>
+          <t>Brave New World</t>
         </is>
       </c>
     </row>
@@ -1065,7 +1065,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>War and Peace</t>
+          <t>The Count of Monte Cristo</t>
         </is>
       </c>
     </row>
@@ -1077,7 +1077,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Jane Eyre</t>
+          <t>Wuthering Heights</t>
         </is>
       </c>
     </row>
@@ -1089,7 +1089,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Wuthering Heights</t>
+          <t>The Grapes of Wrath</t>
         </is>
       </c>
     </row>
@@ -1101,7 +1101,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Pride and Prejudice</t>
+          <t>The Picture of Dorian Gray</t>
         </is>
       </c>
     </row>
@@ -1113,7 +1113,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>The Count of Monte Cristo</t>
+          <t>Jane Eyre</t>
         </is>
       </c>
     </row>
@@ -1125,31 +1125,31 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>The Catcher in the Rye</t>
+          <t>To Kill a Mockingbird</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
         <is>
-          <t>Creative Work</t>
+          <t>Event</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Life of Pi</t>
+          <t>The End of the Mongol Empire</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
         <is>
-          <t>Creative Work</t>
+          <t>Event</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>The Handmaid's Tale</t>
+          <t>The Spanish Conquest of the Aztecs</t>
         </is>
       </c>
     </row>
@@ -1161,7 +1161,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>The Execution of King Louis XVI</t>
+          <t>The Battle of Gettysburg</t>
         </is>
       </c>
     </row>
@@ -1173,7 +1173,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>The Building of the Pyramids of Egypt</t>
+          <t>The Battle of Hastings</t>
         </is>
       </c>
     </row>
@@ -1185,7 +1185,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>French Revolution</t>
+          <t>The Execution of King Louis XVI</t>
         </is>
       </c>
     </row>
@@ -1197,7 +1197,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>The D-Day Invasion</t>
+          <t>English Civil War</t>
         </is>
       </c>
     </row>
@@ -1209,7 +1209,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>The Battle of Gettysburg</t>
+          <t>The Partition of India and Pakistan</t>
         </is>
       </c>
     </row>
@@ -1221,7 +1221,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>The Spanish Conquest of the Aztecs</t>
+          <t>The 9/11 Attacks</t>
         </is>
       </c>
     </row>
@@ -1233,7 +1233,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>The Haitian Revolution</t>
+          <t>The Battle of Midway</t>
         </is>
       </c>
     </row>
@@ -1245,7 +1245,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>The Trial of Galileo</t>
+          <t>The Establishment of the Ming Dynasty</t>
         </is>
       </c>
     </row>
@@ -1257,7 +1257,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>The Establishment of the Ming Dynasty</t>
+          <t>The Discovery of Penicillin</t>
         </is>
       </c>
     </row>
@@ -1269,7 +1269,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>The Vietnam War</t>
+          <t>The Rise of Nazi Germany</t>
         </is>
       </c>
     </row>
@@ -1281,7 +1281,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Signing of the Magna Carta</t>
+          <t>The Surrender of Japan in WWII</t>
         </is>
       </c>
     </row>
@@ -1293,7 +1293,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>The Fall of the Berlin Wall</t>
+          <t>The D-Day Invasion</t>
         </is>
       </c>
     </row>
@@ -1305,7 +1305,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>World War II</t>
+          <t>The Renaissance</t>
         </is>
       </c>
     </row>
@@ -1317,7 +1317,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>The Founding of the United States of America</t>
+          <t>Fall of Constantinople</t>
         </is>
       </c>
     </row>
@@ -1329,7 +1329,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>The Collapse of the Soviet Union</t>
+          <t>The French and Indian War</t>
         </is>
       </c>
     </row>
@@ -1341,7 +1341,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Fall of Constantinople</t>
+          <t>The Emancipation Proclamation</t>
         </is>
       </c>
     </row>
@@ -1353,7 +1353,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>American Civil War</t>
+          <t>Protestant Reformation</t>
         </is>
       </c>
     </row>
@@ -1365,7 +1365,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>The French and Indian War</t>
+          <t>The Establishment of the People's Republic of China</t>
         </is>
       </c>
     </row>
@@ -1377,7 +1377,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>The Cold War</t>
+          <t>Civil Rights Movement</t>
         </is>
       </c>
     </row>
@@ -1389,7 +1389,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>The Battle of Hastings</t>
+          <t>The Battle of Waterloo</t>
         </is>
       </c>
     </row>
@@ -1401,7 +1401,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>The Montgomery Bus Boycott</t>
+          <t>French Revolution</t>
         </is>
       </c>
     </row>
@@ -1413,7 +1413,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>The Emancipation Proclamation</t>
+          <t>The Taiping Rebellion</t>
         </is>
       </c>
     </row>
@@ -1425,7 +1425,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>The Establishment of the People's Republic of China</t>
+          <t>The Assassination of John F. Kennedy</t>
         </is>
       </c>
     </row>
@@ -1437,7 +1437,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>The Battle of Thermopylae</t>
+          <t>The Assassination of Julius Caesar</t>
         </is>
       </c>
     </row>
@@ -1449,103 +1449,103 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>The Boston Tea Party</t>
+          <t>Signing of the Magna Carta</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="inlineStr">
         <is>
-          <t>Language</t>
+          <t>Event</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Russian</t>
+          <t>The Collapse of the Soviet Union</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="inlineStr">
         <is>
-          <t>Language</t>
+          <t>Event</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Greek</t>
+          <t>The Battle of Thermopylae</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="inlineStr">
         <is>
-          <t>Language</t>
+          <t>Event</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>English</t>
+          <t>The End of Apartheid in South Africa</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="inlineStr">
         <is>
-          <t>Language</t>
+          <t>Event</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Turkish</t>
+          <t>American Revolution</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="inlineStr">
         <is>
-          <t>Language</t>
+          <t>Event</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Korean</t>
+          <t>The Founding of the United States of America</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="inlineStr">
         <is>
-          <t>Language</t>
+          <t>Event</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Dutch</t>
+          <t>The Boston Tea Party</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="inlineStr">
         <is>
-          <t>Language</t>
+          <t>Event</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>French</t>
+          <t>American Civil War</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="inlineStr">
         <is>
-          <t>Language</t>
+          <t>Event</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Malay</t>
+          <t>The Discovery of the New World by the Vikings</t>
         </is>
       </c>
     </row>
@@ -1557,7 +1557,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Afrikaans</t>
+          <t>Hebrew</t>
         </is>
       </c>
     </row>
@@ -1569,7 +1569,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Polish</t>
+          <t>Spanish</t>
         </is>
       </c>
     </row>
@@ -1581,7 +1581,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Portuguese</t>
+          <t>Nepali</t>
         </is>
       </c>
     </row>
@@ -1593,7 +1593,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Thai</t>
+          <t>Dutch</t>
         </is>
       </c>
     </row>
@@ -1605,7 +1605,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Gujarati</t>
+          <t>Burmese</t>
         </is>
       </c>
     </row>
@@ -1617,7 +1617,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Kazakh</t>
+          <t>English</t>
         </is>
       </c>
     </row>
@@ -1629,7 +1629,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>German</t>
+          <t>Sinhala</t>
         </is>
       </c>
     </row>
@@ -1641,7 +1641,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Punjabi</t>
+          <t>Romanian</t>
         </is>
       </c>
     </row>
@@ -1653,7 +1653,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Ukrainian</t>
+          <t>Russian</t>
         </is>
       </c>
     </row>
@@ -1665,7 +1665,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Tamil</t>
+          <t>Kazakh</t>
         </is>
       </c>
     </row>
@@ -1677,7 +1677,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Swahili</t>
+          <t>German</t>
         </is>
       </c>
     </row>
@@ -1689,7 +1689,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Hebrew</t>
+          <t>Greek</t>
         </is>
       </c>
     </row>
@@ -1701,7 +1701,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Japanese</t>
+          <t>Afrikaans</t>
         </is>
       </c>
     </row>
@@ -1713,91 +1713,91 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Sinhala</t>
+          <t>Ukrainian</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="inlineStr">
         <is>
-          <t>Organization</t>
+          <t>Language</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Bill &amp; Melinda Gates Foundation</t>
+          <t>Polish</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="inlineStr">
         <is>
-          <t>Organization</t>
+          <t>Language</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Red Cross</t>
+          <t>Haitian Creole</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="inlineStr">
         <is>
-          <t>Organization</t>
+          <t>Language</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>The ACLU</t>
+          <t>Italian</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="inlineStr">
         <is>
-          <t>Organization</t>
+          <t>Language</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Human Rights Watch</t>
+          <t>Swedish</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="inlineStr">
         <is>
-          <t>Organization</t>
+          <t>Language</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>The Salvation Army</t>
+          <t>Thai</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="inlineStr">
         <is>
-          <t>Organization</t>
+          <t>Language</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Charity: Water</t>
+          <t>Portuguese</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="inlineStr">
         <is>
-          <t>Organization</t>
+          <t>Language</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Amnesty International</t>
+          <t>French</t>
         </is>
       </c>
     </row>
@@ -1809,7 +1809,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>National Public Radio</t>
+          <t>UNICEF</t>
         </is>
       </c>
     </row>
@@ -1821,7 +1821,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>World Vision</t>
+          <t>The Carter Center</t>
         </is>
       </c>
     </row>
@@ -1845,7 +1845,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>UNICEF</t>
+          <t>Amnesty International</t>
         </is>
       </c>
     </row>
@@ -1857,7 +1857,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Spotify</t>
+          <t>Red Cross</t>
         </is>
       </c>
     </row>
@@ -1869,7 +1869,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Sony</t>
+          <t>Spotify</t>
         </is>
       </c>
     </row>
@@ -1881,7 +1881,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Volkswagen Group</t>
+          <t>Uber</t>
         </is>
       </c>
     </row>
@@ -1893,7 +1893,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Starbucks</t>
+          <t>Coca-Cola</t>
         </is>
       </c>
     </row>
@@ -1905,7 +1905,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Amazon</t>
+          <t>Toyota</t>
         </is>
       </c>
     </row>
@@ -1917,7 +1917,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Disney</t>
+          <t>Amazon</t>
         </is>
       </c>
     </row>
@@ -1929,7 +1929,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Airbnb</t>
+          <t>Disney</t>
         </is>
       </c>
     </row>
@@ -1941,7 +1941,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Alibaba</t>
+          <t>Johnson &amp; Johnson</t>
         </is>
       </c>
     </row>
@@ -1965,7 +1965,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Uber</t>
+          <t>Walmart</t>
         </is>
       </c>
     </row>
@@ -1977,7 +1977,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>Huawei</t>
         </is>
       </c>
     </row>
@@ -1989,7 +1989,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Huawei</t>
+          <t>Nestlé</t>
         </is>
       </c>
     </row>
@@ -2001,7 +2001,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Walmart</t>
+          <t>Alibaba</t>
         </is>
       </c>
     </row>
@@ -2013,7 +2013,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Walt Disney Company</t>
+          <t>Airbnb</t>
         </is>
       </c>
     </row>
@@ -2025,7 +2025,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>PepsiCo</t>
+          <t>Sony</t>
         </is>
       </c>
     </row>
@@ -2037,7 +2037,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>University of Melbourne</t>
+          <t>Walt Disney Company</t>
         </is>
       </c>
     </row>
@@ -2049,7 +2049,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>California Institute of Technology</t>
+          <t>Bayer</t>
         </is>
       </c>
     </row>
@@ -2061,211 +2061,211 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>ETH Zurich</t>
+          <t>Lund University</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="1" t="inlineStr">
         <is>
-          <t>Organization</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Yale University</t>
+          <t>Cleopatra VII</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="1" t="inlineStr">
         <is>
-          <t>Organization</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>Lund University</t>
+          <t>Socrates</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="1" t="inlineStr">
         <is>
-          <t>Organization</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>University of São Paulo</t>
+          <t>Franklin D. Roosevelt</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="1" t="inlineStr">
         <is>
-          <t>Organization</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Indian Institute of Technology Bombay</t>
+          <t>Vincent van Gogh</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="1" t="inlineStr">
         <is>
-          <t>Organization</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>University of Cambridge</t>
+          <t>Elvis Presley</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="1" t="inlineStr">
         <is>
-          <t>Organization</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Massachusetts Institute of Technology</t>
+          <t>Marie Antoinette</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="1" t="inlineStr">
         <is>
-          <t>Organization</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>University of Sydney</t>
+          <t>William Shakespeare</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="1" t="inlineStr">
         <is>
-          <t>Organization</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Purdue University</t>
+          <t>Leonardo da Vinci</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="1" t="inlineStr">
         <is>
-          <t>Organization</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Australian National University</t>
+          <t>George Washington</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="1" t="inlineStr">
         <is>
-          <t>Organization</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>University of Toronto</t>
+          <t>Isaac Newton</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="1" t="inlineStr">
         <is>
-          <t>Organization</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>University of Delhi</t>
+          <t>Emmeline Pankhurst</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="1" t="inlineStr">
         <is>
-          <t>Organization</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>McGill University</t>
+          <t>Thomas Jefferson</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="1" t="inlineStr">
         <is>
-          <t>Organization</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>University of Tokyo</t>
+          <t>Cleopatra</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="1" t="inlineStr">
         <is>
-          <t>Organization</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>University of Buenos Aires</t>
+          <t>Karl Marx</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="1" t="inlineStr">
         <is>
-          <t>Organization</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>Harvard University</t>
+          <t>Frida Kahlo</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="1" t="inlineStr">
         <is>
-          <t>Organization</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Seoul National University</t>
+          <t>Machiavelli</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="1" t="inlineStr">
         <is>
-          <t>Organization</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>University of California, Berkeley</t>
+          <t>Charles Darwin</t>
         </is>
       </c>
     </row>
@@ -2277,7 +2277,7 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>Thomas Jefferson</t>
+          <t>Julius Caesar</t>
         </is>
       </c>
     </row>
@@ -2289,7 +2289,7 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>Che Guevara</t>
+          <t>Michael Jackson</t>
         </is>
       </c>
     </row>
@@ -2301,7 +2301,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>Florence Nightingale</t>
+          <t>Theodore Roosevelt</t>
         </is>
       </c>
     </row>
@@ -2313,7 +2313,7 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>William Shakespeare</t>
+          <t>Plato</t>
         </is>
       </c>
     </row>
@@ -2325,7 +2325,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Elvis Presley</t>
+          <t>Albert Einstein</t>
         </is>
       </c>
     </row>
@@ -2337,7 +2337,7 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Frida Kahlo</t>
+          <t>Mother Teresa</t>
         </is>
       </c>
     </row>
@@ -2349,7 +2349,7 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>Cleopatra VII</t>
+          <t>Vladimir Lenin</t>
         </is>
       </c>
     </row>
@@ -2373,223 +2373,223 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Leonardo da Vinci</t>
+          <t>Ada Lovelace</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="1" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Species</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>Charles Dickens</t>
+          <t>octopus</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="1" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Species</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Susan B. Anthony</t>
+          <t>tiger</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="1" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Species</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>Napoleon Bonaparte</t>
+          <t>panda</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="1" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Species</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Eleanor Roosevelt</t>
+          <t>harpy eagle</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="1" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Species</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Vincent van Gogh</t>
+          <t>hedgehog</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="1" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Species</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Plato</t>
+          <t>red-shouldered hawk</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="1" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Species</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Julius Caesar</t>
+          <t>cuttlefish</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="1" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Species</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Joan of Arc</t>
+          <t>nile crocodile</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="1" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Species</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>George Washington</t>
+          <t>red-eyed tree frog</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="1" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Species</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Confucius</t>
+          <t>whale shark</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="1" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Species</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Albert Einstein</t>
+          <t>bald eagle</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="1" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Species</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Karl Marx</t>
+          <t>tasmanian devil</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="1" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Species</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Emmeline Pankhurst</t>
+          <t>chameleon</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="1" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Species</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Machiavelli</t>
+          <t>caiman</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="1" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Species</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Socrates</t>
+          <t>bengal tiger</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="1" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Species</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Charles Darwin</t>
+          <t>great horned owl</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="1" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Species</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Theodore Roosevelt</t>
+          <t>snow leopard</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="1" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Species</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Ada Lovelace</t>
+          <t>cheetah</t>
         </is>
       </c>
     </row>
@@ -2601,7 +2601,7 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>praying mantis</t>
+          <t>african wild dog</t>
         </is>
       </c>
     </row>
@@ -2613,7 +2613,7 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>crocodile</t>
+          <t>giant panda</t>
         </is>
       </c>
     </row>
@@ -2625,7 +2625,7 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>panda</t>
+          <t>jaguar</t>
         </is>
       </c>
     </row>
@@ -2637,7 +2637,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>great white shark</t>
+          <t>indian star tortoise</t>
         </is>
       </c>
     </row>
@@ -2649,7 +2649,7 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>caiman</t>
+          <t>wolf</t>
         </is>
       </c>
     </row>
@@ -2661,7 +2661,7 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>bison</t>
+          <t>sloth</t>
         </is>
       </c>
     </row>
@@ -2673,187 +2673,7 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>mantis shrimp</t>
-        </is>
-      </c>
-    </row>
-    <row r="188">
-      <c r="A188" s="1" t="inlineStr">
-        <is>
-          <t>Species</t>
-        </is>
-      </c>
-      <c r="B188" t="inlineStr">
-        <is>
-          <t>komodo dragon</t>
-        </is>
-      </c>
-    </row>
-    <row r="189">
-      <c r="A189" s="1" t="inlineStr">
-        <is>
-          <t>Species</t>
-        </is>
-      </c>
-      <c r="B189" t="inlineStr">
-        <is>
-          <t>lion</t>
-        </is>
-      </c>
-    </row>
-    <row r="190">
-      <c r="A190" s="1" t="inlineStr">
-        <is>
-          <t>Species</t>
-        </is>
-      </c>
-      <c r="B190" t="inlineStr">
-        <is>
-          <t>king cobra</t>
-        </is>
-      </c>
-    </row>
-    <row r="191">
-      <c r="A191" s="1" t="inlineStr">
-        <is>
-          <t>Species</t>
-        </is>
-      </c>
-      <c r="B191" t="inlineStr">
-        <is>
-          <t>giant panda</t>
-        </is>
-      </c>
-    </row>
-    <row r="192">
-      <c r="A192" s="1" t="inlineStr">
-        <is>
-          <t>Species</t>
-        </is>
-      </c>
-      <c r="B192" t="inlineStr">
-        <is>
-          <t>sloth</t>
-        </is>
-      </c>
-    </row>
-    <row r="193">
-      <c r="A193" s="1" t="inlineStr">
-        <is>
-          <t>Species</t>
-        </is>
-      </c>
-      <c r="B193" t="inlineStr">
-        <is>
-          <t>hedgehog</t>
-        </is>
-      </c>
-    </row>
-    <row r="194">
-      <c r="A194" s="1" t="inlineStr">
-        <is>
-          <t>Species</t>
-        </is>
-      </c>
-      <c r="B194" t="inlineStr">
-        <is>
-          <t>bengal tiger</t>
-        </is>
-      </c>
-    </row>
-    <row r="195">
-      <c r="A195" s="1" t="inlineStr">
-        <is>
-          <t>Species</t>
-        </is>
-      </c>
-      <c r="B195" t="inlineStr">
-        <is>
           <t>wolverine</t>
-        </is>
-      </c>
-    </row>
-    <row r="196">
-      <c r="A196" s="1" t="inlineStr">
-        <is>
-          <t>Species</t>
-        </is>
-      </c>
-      <c r="B196" t="inlineStr">
-        <is>
-          <t>great horned owl</t>
-        </is>
-      </c>
-    </row>
-    <row r="197">
-      <c r="A197" s="1" t="inlineStr">
-        <is>
-          <t>Species</t>
-        </is>
-      </c>
-      <c r="B197" t="inlineStr">
-        <is>
-          <t>bald eagle</t>
-        </is>
-      </c>
-    </row>
-    <row r="198">
-      <c r="A198" s="1" t="inlineStr">
-        <is>
-          <t>Species</t>
-        </is>
-      </c>
-      <c r="B198" t="inlineStr">
-        <is>
-          <t>chameleon</t>
-        </is>
-      </c>
-    </row>
-    <row r="199">
-      <c r="A199" s="1" t="inlineStr">
-        <is>
-          <t>Species</t>
-        </is>
-      </c>
-      <c r="B199" t="inlineStr">
-        <is>
-          <t>jaguar</t>
-        </is>
-      </c>
-    </row>
-    <row r="200">
-      <c r="A200" s="1" t="inlineStr">
-        <is>
-          <t>Species</t>
-        </is>
-      </c>
-      <c r="B200" t="inlineStr">
-        <is>
-          <t>tiger</t>
-        </is>
-      </c>
-    </row>
-    <row r="201">
-      <c r="A201" s="1" t="inlineStr">
-        <is>
-          <t>Species</t>
-        </is>
-      </c>
-      <c r="B201" t="inlineStr">
-        <is>
-          <t>pygmy hippo</t>
-        </is>
-      </c>
-    </row>
-    <row r="202">
-      <c r="A202" s="1" t="inlineStr">
-        <is>
-          <t>Species</t>
-        </is>
-      </c>
-      <c r="B202" t="inlineStr">
-        <is>
-          <t>red-shouldered hawk</t>
         </is>
       </c>
     </row>

</xml_diff>